<commit_message>
Rudder step motor using Timer1
</commit_message>
<xml_diff>
--- a/doc/boat connection.xlsx
+++ b/doc/boat connection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\boat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E8897A-03B2-4049-9D69-E75C8F713C25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E556D2-6D62-4AE8-8AD5-6D7724D576CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E3A2800-F707-4B86-9CC8-DB3F839EA1A1}"/>
+    <workbookView xWindow="5715" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{9E3A2800-F707-4B86-9CC8-DB3F839EA1A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>PB0</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Motor PWM</t>
+  </si>
+  <si>
+    <t>Rudder Step Motor</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +592,7 @@
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,6 +656,9 @@
       <c r="G5" t="s">
         <v>37</v>
       </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Radio module working but no RF
</commit_message>
<xml_diff>
--- a/doc/boat connection.xlsx
+++ b/doc/boat connection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\boat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E556D2-6D62-4AE8-8AD5-6D7724D576CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3F38AF-CDBD-4A97-A2BD-31A6C6AD6566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{9E3A2800-F707-4B86-9CC8-DB3F839EA1A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E3A2800-F707-4B86-9CC8-DB3F839EA1A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <t>PB0</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>Rudder Step Motor</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>PD2/INT0</t>
+  </si>
+  <si>
+    <t>PD3/INT1</t>
+  </si>
+  <si>
+    <t>Radio IRQ</t>
+  </si>
+  <si>
+    <t>Radio CE</t>
+  </si>
+  <si>
+    <t>Radio CSN</t>
   </si>
 </sst>
 </file>
@@ -582,7 +600,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +708,9 @@
       <c r="G7" t="s">
         <v>39</v>
       </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -698,14 +719,14 @@
       <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
       <c r="F8" t="s">
         <v>53</v>
       </c>
       <c r="G8" t="s">
         <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -724,6 +745,9 @@
       <c r="G9" t="s">
         <v>41</v>
       </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -879,30 +903,42 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
       <c r="G22" t="s">
         <v>30</v>
       </c>
+      <c r="H22" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
       <c r="F23" t="s">
         <v>11</v>
       </c>
       <c r="G23" t="s">
         <v>31</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,11 +948,17 @@
       <c r="B24" t="s">
         <v>32</v>
       </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
       <c r="F24" t="s">
         <v>12</v>
       </c>
       <c r="G24" t="s">
         <v>32</v>
+      </c>
+      <c r="H24" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Radio working, but have interference
</commit_message>
<xml_diff>
--- a/doc/boat connection.xlsx
+++ b/doc/boat connection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\boat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3F38AF-CDBD-4A97-A2BD-31A6C6AD6566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C388AB50-8291-4B6B-8964-64DFD958D32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E3A2800-F707-4B86-9CC8-DB3F839EA1A1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
   <si>
     <t>PB0</t>
   </si>
@@ -246,6 +246,21 @@
   </si>
   <si>
     <t>Radio CSN</t>
+  </si>
+  <si>
+    <t>TRF_DR1</t>
+  </si>
+  <si>
+    <t>TRF_CE</t>
+  </si>
+  <si>
+    <t>TRF_CS</t>
+  </si>
+  <si>
+    <t>TRF_CLK1</t>
+  </si>
+  <si>
+    <t>TRF_DATA1</t>
   </si>
 </sst>
 </file>
@@ -597,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E6B6CA-A0DD-4C56-904F-2A2E64AE780B}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,9 +626,10 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -621,7 +637,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -641,7 +657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -658,7 +674,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -678,7 +694,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -692,7 +708,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -712,13 +728,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
       <c r="F8" t="s">
         <v>53</v>
       </c>
@@ -728,8 +747,11 @@
       <c r="H8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -748,8 +770,11 @@
       <c r="H9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -763,7 +788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -777,7 +802,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -791,7 +816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -805,7 +830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -819,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -836,7 +861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -853,7 +878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -873,7 +898,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -887,7 +912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -901,7 +926,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -920,8 +945,11 @@
       <c r="H22" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -940,8 +968,11 @@
       <c r="H23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -960,8 +991,11 @@
       <c r="H24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -978,7 +1012,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -995,7 +1029,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1046,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>

</xml_diff>